<commit_message>
completed 1st draft of Ch 3
</commit_message>
<xml_diff>
--- a/Book Schedule.xlsx
+++ b/Book Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Packt - Psh 7.2 + Srv 2022\PacktPS72\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{904AB0F0-A22C-4015-8BF2-250800DE29B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF0A9E1-DF1D-4E3A-90A6-480F88681350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7725" yWindow="2805" windowWidth="21600" windowHeight="12645" xr2:uid="{6C5F0C63-7165-44B9-851C-3F7532245ECC}"/>
+    <workbookView xWindow="29685" yWindow="3570" windowWidth="21600" windowHeight="12645" xr2:uid="{6C5F0C63-7165-44B9-851C-3F7532245ECC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +124,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -140,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -149,6 +155,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -468,7 +477,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,6 +548,13 @@
       <c r="E3" s="2">
         <v>44680</v>
       </c>
+      <c r="F3" s="2">
+        <v>44681</v>
+      </c>
+      <c r="G3" s="4">
+        <f>F3-E3</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -552,6 +568,13 @@
       </c>
       <c r="E4" s="2">
         <v>44692</v>
+      </c>
+      <c r="F4" s="2">
+        <v>44683</v>
+      </c>
+      <c r="G4" s="3">
+        <f>F4-E4</f>
+        <v>-9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ch 4 first draft
</commit_message>
<xml_diff>
--- a/Book Schedule.xlsx
+++ b/Book Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Packt - Psh 7.2 + Srv 2022\PacktPS72\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF0A9E1-DF1D-4E3A-90A6-480F88681350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B418952-739E-49DB-916E-5D0746E8F952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29685" yWindow="3570" windowWidth="21600" windowHeight="12645" xr2:uid="{6C5F0C63-7165-44B9-851C-3F7532245ECC}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H16" sqref="A1:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,13 +582,20 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2">
         <v>44704</v>
+      </c>
+      <c r="F5" s="2">
+        <v>44690</v>
+      </c>
+      <c r="G5" s="3">
+        <f>F5-E5</f>
+        <v>-14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -596,10 +603,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E6" s="2">
         <v>44716</v>

</xml_diff>